<commit_message>
tabled results day 200
</commit_message>
<xml_diff>
--- a/results/featureextraction.xlsx
+++ b/results/featureextraction.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="69">
   <si>
     <t>id</t>
   </si>
@@ -91,6 +91,42 @@
     <t>MLP7D050FB2</t>
   </si>
   <si>
+    <t>MLP7D070FA</t>
+  </si>
+  <si>
+    <t>MLP7D070FC1</t>
+  </si>
+  <si>
+    <t>MLP7D070FC2</t>
+  </si>
+  <si>
+    <t>MLP7D070FD</t>
+  </si>
+  <si>
+    <t>MLP7D070FB1</t>
+  </si>
+  <si>
+    <t>MLP7D070FB2</t>
+  </si>
+  <si>
+    <t>MLP7D0100FA</t>
+  </si>
+  <si>
+    <t>MLP7D0100FC1</t>
+  </si>
+  <si>
+    <t>MLP7D0100FC2</t>
+  </si>
+  <si>
+    <t>MLP7D0100FD</t>
+  </si>
+  <si>
+    <t>MLP7D0100FB1</t>
+  </si>
+  <si>
+    <t>MLP7D0100FB2</t>
+  </si>
+  <si>
     <t>MLP8D030FA</t>
   </si>
   <si>
@@ -125,6 +161,42 @@
   </si>
   <si>
     <t>MLP8D050FB2</t>
+  </si>
+  <si>
+    <t>MLP8D070FA</t>
+  </si>
+  <si>
+    <t>MLP8D070FC1</t>
+  </si>
+  <si>
+    <t>MLP8D070FC2</t>
+  </si>
+  <si>
+    <t>MLP8D070FD</t>
+  </si>
+  <si>
+    <t>MLP8D070FB1</t>
+  </si>
+  <si>
+    <t>MLP8D070FB2</t>
+  </si>
+  <si>
+    <t>MLP8D0100FA</t>
+  </si>
+  <si>
+    <t>MLP8D0100FC1</t>
+  </si>
+  <si>
+    <t>MLP8D0100FC2</t>
+  </si>
+  <si>
+    <t>MLP8D0100FD</t>
+  </si>
+  <si>
+    <t>MLP8D0100FB1</t>
+  </si>
+  <si>
+    <t>MLP8D0100FB2</t>
   </si>
   <si>
     <t>mlp</t>
@@ -506,7 +578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,7 +633,7 @@
         <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D2">
         <v>7</v>
@@ -573,25 +645,25 @@
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>6.806822694360894</v>
+        <v>10.00438495730581</v>
       </c>
       <c r="K2">
-        <v>6.642316262693514</v>
+        <v>10.38203207073011</v>
       </c>
       <c r="L2">
-        <v>4.529231764425013</v>
+        <v>6.229437798360602</v>
       </c>
       <c r="M2">
-        <v>4.808145816958726</v>
+        <v>7.156459310618192</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -602,7 +674,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D3">
         <v>7</v>
@@ -614,25 +686,25 @@
         <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.9765347210620801</v>
+        <v>1.024213017200579</v>
       </c>
       <c r="K3">
-        <v>0.9945797382199946</v>
+        <v>1.088744493830769</v>
       </c>
       <c r="L3">
-        <v>0.6909591072944891</v>
+        <v>0.7320699560549179</v>
       </c>
       <c r="M3">
-        <v>0.7400462883946674</v>
+        <v>0.7690979236193421</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -643,7 +715,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D4">
         <v>7</v>
@@ -655,25 +727,25 @@
         <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="J4">
-        <v>2.38783587012368</v>
+        <v>2.544768190940791</v>
       </c>
       <c r="K4">
-        <v>2.272826937587504</v>
+        <v>2.448388180642767</v>
       </c>
       <c r="L4">
-        <v>1.855427327412968</v>
+        <v>1.987230862870438</v>
       </c>
       <c r="M4">
-        <v>1.816435888062654</v>
+        <v>1.939582945501945</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -684,7 +756,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>7</v>
@@ -696,7 +768,7 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -705,19 +777,19 @@
         <v>500</v>
       </c>
       <c r="J5">
-        <v>1.053424905759508</v>
+        <v>1.159082154418196</v>
       </c>
       <c r="K5">
-        <v>1.00991750178233</v>
+        <v>1.15848033671324</v>
       </c>
       <c r="L5">
-        <v>0.6680375266727566</v>
+        <v>0.7279445011687906</v>
       </c>
       <c r="M5">
-        <v>0.6733407335909875</v>
+        <v>0.7466168809686057</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -728,7 +800,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D6">
         <v>7</v>
@@ -740,7 +812,7 @@
         <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -749,19 +821,19 @@
         <v>10000</v>
       </c>
       <c r="J6">
-        <v>0.5586115717887878</v>
+        <v>0.5641677379608154</v>
       </c>
       <c r="K6">
-        <v>0.7918316125869751</v>
+        <v>0.7866249084472656</v>
       </c>
       <c r="L6">
-        <v>0.3268327116966248</v>
+        <v>0.3388946056365967</v>
       </c>
       <c r="M6">
-        <v>0.4895786345005035</v>
+        <v>0.4874206483364105</v>
       </c>
       <c r="N6" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -772,7 +844,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -784,28 +856,28 @@
         <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="J7">
-        <v>1.328913807868958</v>
+        <v>1.226793766021728</v>
       </c>
       <c r="K7">
-        <v>1.197025656700134</v>
+        <v>1.124013423919678</v>
       </c>
       <c r="L7">
-        <v>0.9754370450973512</v>
+        <v>0.8919517397880554</v>
       </c>
       <c r="M7">
-        <v>0.8744686841964722</v>
+        <v>0.8031153678894043</v>
       </c>
       <c r="N7" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -816,7 +888,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -828,25 +900,25 @@
         <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="J8">
-        <v>9.887994377805267</v>
+        <v>8.742085295754011</v>
       </c>
       <c r="K8">
-        <v>9.869731813203066</v>
+        <v>7.005193112891305</v>
       </c>
       <c r="L8">
-        <v>6.047038020966431</v>
+        <v>5.508570743702134</v>
       </c>
       <c r="M8">
-        <v>7.053567669359833</v>
+        <v>5.306436106149635</v>
       </c>
       <c r="N8" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -857,7 +929,7 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -869,25 +941,25 @@
         <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>1.031974750629558</v>
+        <v>1.073110079746259</v>
       </c>
       <c r="K9">
-        <v>1.045120318108673</v>
+        <v>1.524892736118029</v>
       </c>
       <c r="L9">
-        <v>0.7470197177001958</v>
+        <v>0.760928391182911</v>
       </c>
       <c r="M9">
-        <v>0.7494539170371877</v>
+        <v>0.8332226603483276</v>
       </c>
       <c r="N9" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -898,7 +970,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D10">
         <v>7</v>
@@ -910,25 +982,25 @@
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>2.709802020956094</v>
+        <v>2.39563593848303</v>
       </c>
       <c r="K10">
-        <v>2.592831443213211</v>
+        <v>2.39395333352028</v>
       </c>
       <c r="L10">
-        <v>2.200454683114258</v>
+        <v>1.80416292422677</v>
       </c>
       <c r="M10">
-        <v>2.156031239554435</v>
+        <v>1.806866226519419</v>
       </c>
       <c r="N10" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -939,7 +1011,7 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D11">
         <v>7</v>
@@ -951,7 +1023,7 @@
         <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -960,19 +1032,19 @@
         <v>500</v>
       </c>
       <c r="J11">
-        <v>1.359709211284885</v>
+        <v>1.274157232410373</v>
       </c>
       <c r="K11">
-        <v>1.160333578767926</v>
+        <v>1.144000486287242</v>
       </c>
       <c r="L11">
-        <v>0.8907599215037545</v>
+        <v>0.8368238400344931</v>
       </c>
       <c r="M11">
-        <v>0.7822903859689619</v>
+        <v>0.7557077598964967</v>
       </c>
       <c r="N11" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -983,7 +1055,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D12">
         <v>7</v>
@@ -995,7 +1067,7 @@
         <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1004,19 +1076,19 @@
         <v>10000</v>
       </c>
       <c r="J12">
-        <v>0.5539144277572632</v>
+        <v>0.5582820773124695</v>
       </c>
       <c r="K12">
-        <v>0.7751167416572571</v>
+        <v>0.7796034812927246</v>
       </c>
       <c r="L12">
-        <v>0.3293488919734955</v>
+        <v>0.3302969038486481</v>
       </c>
       <c r="M12">
-        <v>0.4926495552062988</v>
+        <v>0.4906741976737976</v>
       </c>
       <c r="N12" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1027,7 +1099,7 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D13">
         <v>7</v>
@@ -1039,28 +1111,28 @@
         <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="J13">
-        <v>1.509628534317017</v>
+        <v>1.409807443618774</v>
       </c>
       <c r="K13">
-        <v>1.345777988433838</v>
+        <v>1.280019998550415</v>
       </c>
       <c r="L13">
-        <v>1.092472434043884</v>
+        <v>1.020635366439819</v>
       </c>
       <c r="M13">
-        <v>0.9719778895378112</v>
+        <v>0.8993344306945801</v>
       </c>
       <c r="N13" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1071,37 +1143,37 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14">
         <v>5</v>
       </c>
       <c r="F14">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="J14">
-        <v>4.266380459085286</v>
+        <v>8.762072914433613</v>
       </c>
       <c r="K14">
-        <v>4.179572875339118</v>
+        <v>7.156006714489902</v>
       </c>
       <c r="L14">
-        <v>3.026725945272313</v>
+        <v>5.438984149459307</v>
       </c>
       <c r="M14">
-        <v>3.072167592494359</v>
+        <v>5.243360452543156</v>
       </c>
       <c r="N14" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1112,37 +1184,37 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>5</v>
       </c>
       <c r="F15">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0.9124141290599435</v>
+        <v>1.075192081739718</v>
       </c>
       <c r="K15">
-        <v>1.01960835733747</v>
+        <v>1.067863340038893</v>
       </c>
       <c r="L15">
-        <v>0.6251250838332668</v>
+        <v>0.7691299407342849</v>
       </c>
       <c r="M15">
-        <v>0.68097221077632</v>
+        <v>0.7812450732794299</v>
       </c>
       <c r="N15" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1153,37 +1225,37 @@
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16">
         <v>5</v>
       </c>
       <c r="F16">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>2.251627581892316</v>
+        <v>2.489847703058245</v>
       </c>
       <c r="K16">
-        <v>2.160071427012375</v>
+        <v>2.408389040725606</v>
       </c>
       <c r="L16">
-        <v>1.6951459251027</v>
+        <v>1.895860299762089</v>
       </c>
       <c r="M16">
-        <v>1.63617710280832</v>
+        <v>1.818543136674192</v>
       </c>
       <c r="N16" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1194,19 +1266,19 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17">
         <v>5</v>
       </c>
       <c r="F17">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1215,19 +1287,19 @@
         <v>500</v>
       </c>
       <c r="J17">
-        <v>0.983841070314279</v>
+        <v>1.202933038419213</v>
       </c>
       <c r="K17">
-        <v>0.9030700659263653</v>
+        <v>1.073148959577262</v>
       </c>
       <c r="L17">
-        <v>0.6027227683454737</v>
+        <v>0.7657352502530212</v>
       </c>
       <c r="M17">
-        <v>0.5933853423059607</v>
+        <v>0.7008879307590117</v>
       </c>
       <c r="N17" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1238,19 +1310,19 @@
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18">
         <v>5</v>
       </c>
       <c r="F18">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1259,19 +1331,19 @@
         <v>10000</v>
       </c>
       <c r="J18">
-        <v>0.5586115717887878</v>
+        <v>0.5569562911987305</v>
       </c>
       <c r="K18">
-        <v>0.7918316125869751</v>
+        <v>0.7641125917434692</v>
       </c>
       <c r="L18">
-        <v>0.3268327116966248</v>
+        <v>0.3302320837974548</v>
       </c>
       <c r="M18">
-        <v>0.4895786345005035</v>
+        <v>0.492600679397583</v>
       </c>
       <c r="N18" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1282,40 +1354,40 @@
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19">
         <v>5</v>
       </c>
       <c r="F19">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="J19">
-        <v>1.328913807868958</v>
+        <v>1.416856050491333</v>
       </c>
       <c r="K19">
-        <v>1.197025656700134</v>
+        <v>1.290968298912048</v>
       </c>
       <c r="L19">
-        <v>0.9754370450973512</v>
+        <v>1.011521100997925</v>
       </c>
       <c r="M19">
-        <v>0.8744686841964722</v>
+        <v>0.9060245752334596</v>
       </c>
       <c r="N19" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1326,37 +1398,37 @@
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>5</v>
       </c>
       <c r="F20">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G20" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="J20">
-        <v>4.646787813206887</v>
+        <v>12.94084420141916</v>
       </c>
       <c r="K20">
-        <v>4.544633378437865</v>
+        <v>13.01063059834415</v>
       </c>
       <c r="L20">
-        <v>3.454716295976118</v>
+        <v>7.970917459785643</v>
       </c>
       <c r="M20">
-        <v>3.5771459391475</v>
+        <v>9.169138302429399</v>
       </c>
       <c r="N20" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1367,37 +1439,37 @@
         <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21">
         <v>5</v>
       </c>
       <c r="F21">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G21" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0.9468838204876603</v>
+        <v>0.9971738669133645</v>
       </c>
       <c r="K21">
-        <v>1.004428920401103</v>
+        <v>0.9692713886289193</v>
       </c>
       <c r="L21">
-        <v>0.6614637154860172</v>
+        <v>0.7037051429335435</v>
       </c>
       <c r="M21">
-        <v>0.708170453712347</v>
+        <v>0.7307312767841569</v>
       </c>
       <c r="N21" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1408,37 +1480,37 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>5</v>
       </c>
       <c r="F22">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G22" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>2.439976685833491</v>
+        <v>2.33936487971967</v>
       </c>
       <c r="K22">
-        <v>2.253236057347103</v>
+        <v>2.080566549116424</v>
       </c>
       <c r="L22">
-        <v>1.921632437089849</v>
+        <v>1.774700128955684</v>
       </c>
       <c r="M22">
-        <v>1.782286349495255</v>
+        <v>1.61815399085998</v>
       </c>
       <c r="N22" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1449,19 +1521,19 @@
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>5</v>
       </c>
       <c r="F23">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1470,19 +1542,19 @@
         <v>500</v>
       </c>
       <c r="J23">
-        <v>1.141499250676306</v>
+        <v>1.175129163110965</v>
       </c>
       <c r="K23">
-        <v>1.144939214754617</v>
+        <v>1.050160316509077</v>
       </c>
       <c r="L23">
-        <v>0.726865811878577</v>
+        <v>0.7447468981295607</v>
       </c>
       <c r="M23">
-        <v>0.752728683583975</v>
+        <v>0.6944530102657764</v>
       </c>
       <c r="N23" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1493,19 +1565,19 @@
         <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24">
         <v>5</v>
       </c>
       <c r="F24">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1514,19 +1586,19 @@
         <v>10000</v>
       </c>
       <c r="J24">
-        <v>0.5539144277572632</v>
+        <v>0.5699505805969238</v>
       </c>
       <c r="K24">
-        <v>0.7751167416572571</v>
+        <v>0.7646061182022095</v>
       </c>
       <c r="L24">
-        <v>0.3293488919734955</v>
+        <v>0.341210275888443</v>
       </c>
       <c r="M24">
-        <v>0.4926495552062988</v>
+        <v>0.4953839182853699</v>
       </c>
       <c r="N24" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1537,40 +1609,1060 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>100</v>
+      </c>
+      <c r="G25" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>40000</v>
+      </c>
+      <c r="J25">
+        <v>1.345978498458862</v>
+      </c>
+      <c r="K25">
+        <v>1.161882996559143</v>
+      </c>
+      <c r="L25">
+        <v>0.9561001062393188</v>
+      </c>
+      <c r="M25">
+        <v>0.8256415128707886</v>
+      </c>
+      <c r="N25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="D25">
+      <c r="C26" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26">
         <v>8</v>
       </c>
-      <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="F25">
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>4.076357498729775</v>
+      </c>
+      <c r="K26">
+        <v>4.020282028847351</v>
+      </c>
+      <c r="L26">
+        <v>2.859452403658219</v>
+      </c>
+      <c r="M26">
+        <v>2.94637327588741</v>
+      </c>
+      <c r="N26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0.9155739817374503</v>
+      </c>
+      <c r="K27">
+        <v>0.9761511657434759</v>
+      </c>
+      <c r="L27">
+        <v>0.6350351691539158</v>
+      </c>
+      <c r="M27">
+        <v>0.711501340255003</v>
+      </c>
+      <c r="N27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>2.237444441309334</v>
+      </c>
+      <c r="K28">
+        <v>2.172132039603001</v>
+      </c>
+      <c r="L28">
+        <v>1.683241308867986</v>
+      </c>
+      <c r="M28">
+        <v>1.621275420525324</v>
+      </c>
+      <c r="N28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29">
+        <v>8</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>500</v>
+      </c>
+      <c r="J29">
+        <v>1.062405375416964</v>
+      </c>
+      <c r="K29">
+        <v>0.9881543907887969</v>
+      </c>
+      <c r="L29">
+        <v>0.6596075763026465</v>
+      </c>
+      <c r="M29">
+        <v>0.6597517434385272</v>
+      </c>
+      <c r="N29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30">
+        <v>8</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>10000</v>
+      </c>
+      <c r="J30">
+        <v>0.5641677379608154</v>
+      </c>
+      <c r="K30">
+        <v>0.7866249084472656</v>
+      </c>
+      <c r="L30">
+        <v>0.3388946056365967</v>
+      </c>
+      <c r="M30">
+        <v>0.4874206483364105</v>
+      </c>
+      <c r="N30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>40000</v>
+      </c>
+      <c r="J31">
+        <v>1.226793766021728</v>
+      </c>
+      <c r="K31">
+        <v>1.124013423919678</v>
+      </c>
+      <c r="L31">
+        <v>0.8919517397880554</v>
+      </c>
+      <c r="M31">
+        <v>0.8031153678894043</v>
+      </c>
+      <c r="N31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
         <v>50</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>5.338728458127044</v>
+      </c>
+      <c r="K32">
+        <v>4.849818498222812</v>
+      </c>
+      <c r="L32">
+        <v>3.612886101434982</v>
+      </c>
+      <c r="M32">
+        <v>3.706538223720009</v>
+      </c>
+      <c r="N32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33">
+        <v>8</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>50</v>
+      </c>
+      <c r="G33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0.9241121725086832</v>
+      </c>
+      <c r="K33">
+        <v>1.022384170889355</v>
+      </c>
+      <c r="L33">
+        <v>0.6391465526727822</v>
+      </c>
+      <c r="M33">
+        <v>0.7169104026314912</v>
+      </c>
+      <c r="N33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34">
+        <v>8</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>50</v>
+      </c>
+      <c r="G34" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>2.214805897512409</v>
+      </c>
+      <c r="K34">
+        <v>2.114792820896836</v>
+      </c>
+      <c r="L34">
+        <v>1.675128446453048</v>
+      </c>
+      <c r="M34">
+        <v>1.593907146675113</v>
+      </c>
+      <c r="N34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>5</v>
+      </c>
+      <c r="F35">
+        <v>50</v>
+      </c>
+      <c r="G35" t="s">
+        <v>65</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>500</v>
+      </c>
+      <c r="J35">
+        <v>1.088334976566296</v>
+      </c>
+      <c r="K35">
+        <v>1.040653311078247</v>
+      </c>
+      <c r="L35">
+        <v>0.6857405132689588</v>
+      </c>
+      <c r="M35">
+        <v>0.6834561486871692</v>
+      </c>
+      <c r="N35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>50</v>
+      </c>
+      <c r="G36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>10000</v>
+      </c>
+      <c r="J36">
+        <v>0.5582820773124695</v>
+      </c>
+      <c r="K36">
+        <v>0.7796034812927246</v>
+      </c>
+      <c r="L36">
+        <v>0.3302969038486481</v>
+      </c>
+      <c r="M36">
+        <v>0.4906741976737976</v>
+      </c>
+      <c r="N36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>50</v>
+      </c>
+      <c r="G37" t="s">
+        <v>67</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>40000</v>
+      </c>
+      <c r="J37">
+        <v>1.409807443618774</v>
+      </c>
+      <c r="K37">
+        <v>1.280019998550415</v>
+      </c>
+      <c r="L37">
+        <v>1.020635366439819</v>
+      </c>
+      <c r="M37">
+        <v>0.8993344306945801</v>
+      </c>
+      <c r="N37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>70</v>
+      </c>
+      <c r="G38" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>4.384159545696203</v>
+      </c>
+      <c r="K38">
+        <v>4.162281584407036</v>
+      </c>
+      <c r="L38">
+        <v>3.181135376681208</v>
+      </c>
+      <c r="M38">
+        <v>3.258335834263824</v>
+      </c>
+      <c r="N38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>70</v>
+      </c>
+      <c r="G39" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0.9120775868373248</v>
+      </c>
+      <c r="K39">
+        <v>1.011216287969775</v>
+      </c>
+      <c r="L39">
+        <v>0.6296546866210083</v>
+      </c>
+      <c r="M39">
+        <v>0.6927480318783719</v>
+      </c>
+      <c r="N39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40">
+        <v>8</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>70</v>
+      </c>
+      <c r="G40" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>2.237837498323704</v>
+      </c>
+      <c r="K40">
+        <v>2.168358710752662</v>
+      </c>
+      <c r="L40">
+        <v>1.65974910282075</v>
+      </c>
+      <c r="M40">
+        <v>1.623729725666519</v>
+      </c>
+      <c r="N40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>70</v>
+      </c>
+      <c r="G41" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>500</v>
+      </c>
+      <c r="J41">
+        <v>1.074766930874451</v>
+      </c>
+      <c r="K41">
+        <v>0.9938047168727726</v>
+      </c>
+      <c r="L41">
+        <v>0.6831228271900771</v>
+      </c>
+      <c r="M41">
+        <v>0.6781311475420246</v>
+      </c>
+      <c r="N41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42">
+        <v>8</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>70</v>
+      </c>
+      <c r="G42" t="s">
+        <v>66</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>10000</v>
+      </c>
+      <c r="J42">
+        <v>0.5569562911987305</v>
+      </c>
+      <c r="K42">
+        <v>0.7641125917434692</v>
+      </c>
+      <c r="L42">
+        <v>0.3302320837974548</v>
+      </c>
+      <c r="M42">
+        <v>0.492600679397583</v>
+      </c>
+      <c r="N42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43">
+        <v>8</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>70</v>
+      </c>
+      <c r="G43" t="s">
+        <v>67</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>40000</v>
+      </c>
+      <c r="J43">
+        <v>1.416856050491333</v>
+      </c>
+      <c r="K43">
+        <v>1.290968298912048</v>
+      </c>
+      <c r="L43">
+        <v>1.011521100997925</v>
+      </c>
+      <c r="M43">
+        <v>0.9060245752334596</v>
+      </c>
+      <c r="N43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C44" t="s">
+        <v>61</v>
+      </c>
+      <c r="D44">
+        <v>8</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>100</v>
+      </c>
+      <c r="G44" t="s">
+        <v>62</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>4.50628340310844</v>
+      </c>
+      <c r="K44">
+        <v>4.328067808803192</v>
+      </c>
+      <c r="L44">
+        <v>3.212188387619715</v>
+      </c>
+      <c r="M44">
+        <v>3.312440959487002</v>
+      </c>
+      <c r="N44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>30000</v>
-      </c>
-      <c r="J25">
-        <v>1.509628534317017</v>
-      </c>
-      <c r="K25">
-        <v>1.345777988433838</v>
-      </c>
-      <c r="L25">
-        <v>1.092472434043884</v>
-      </c>
-      <c r="M25">
-        <v>0.9719778895378112</v>
-      </c>
-      <c r="N25" t="s">
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D45">
+        <v>8</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>100</v>
+      </c>
+      <c r="G45" t="s">
+        <v>63</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0.9610679781078867</v>
+      </c>
+      <c r="K45">
+        <v>0.9746878827125223</v>
+      </c>
+      <c r="L45">
+        <v>0.66444439348795</v>
+      </c>
+      <c r="M45">
+        <v>0.6919813381530229</v>
+      </c>
+      <c r="N45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="1">
         <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46">
+        <v>8</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>100</v>
+      </c>
+      <c r="G46" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>2.298198852714227</v>
+      </c>
+      <c r="K46">
+        <v>2.188262558105474</v>
+      </c>
+      <c r="L46">
+        <v>1.727794571164431</v>
+      </c>
+      <c r="M46">
+        <v>1.664348337943026</v>
+      </c>
+      <c r="N46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47">
+        <v>8</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <v>100</v>
+      </c>
+      <c r="G47" t="s">
+        <v>65</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>500</v>
+      </c>
+      <c r="J47">
+        <v>1.111590758040682</v>
+      </c>
+      <c r="K47">
+        <v>0.9981345886485642</v>
+      </c>
+      <c r="L47">
+        <v>0.6881812032075636</v>
+      </c>
+      <c r="M47">
+        <v>0.6637042234937611</v>
+      </c>
+      <c r="N47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48">
+        <v>8</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>100</v>
+      </c>
+      <c r="G48" t="s">
+        <v>66</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>10000</v>
+      </c>
+      <c r="J48">
+        <v>0.5699505805969238</v>
+      </c>
+      <c r="K48">
+        <v>0.7646061182022095</v>
+      </c>
+      <c r="L48">
+        <v>0.341210275888443</v>
+      </c>
+      <c r="M48">
+        <v>0.4953839182853699</v>
+      </c>
+      <c r="N48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49">
+        <v>8</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
+        <v>100</v>
+      </c>
+      <c r="G49" t="s">
+        <v>67</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>40000</v>
+      </c>
+      <c r="J49">
+        <v>1.345978498458862</v>
+      </c>
+      <c r="K49">
+        <v>1.161882996559143</v>
+      </c>
+      <c r="L49">
+        <v>0.9561001062393188</v>
+      </c>
+      <c r="M49">
+        <v>0.8256415128707886</v>
+      </c>
+      <c r="N49" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>